<commit_message>
Change the output's format
</commit_message>
<xml_diff>
--- a/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
+++ b/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29777435-B08F-3840-9AB0-13868E1F18FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231EBD6C-B790-4944-BF3C-021FBE5DC88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -267,9 +267,6 @@
     <t>COMP 750 Algorithm Analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">COMP  590 &amp; 790- 175   Special Topics: Visual Computing Systems        </t>
-  </si>
-  <si>
     <t>COMP  790 - 158   Special Topics: Special topics in Natural Language Processing</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>COMP 790 - 183 Special Topics: Transfer Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMP 590 &amp; 790-175 Special Topics: Visual Computing Systems        </t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1372,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2034,7 +2034,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -3238,7 +3238,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -3780,7 +3780,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -4073,7 +4073,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4837,7 +4837,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4851,7 +4851,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4964,7 +4964,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5112,7 +5112,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -10305,7 +10305,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10550,7 +10550,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12695,7 +12695,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13240,7 +13240,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -15204,7 +15204,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -15523,7 +15523,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17171,7 +17171,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -18484,7 +18484,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -19797,7 +19797,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -22198,7 +22198,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -24042,7 +24042,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -24704,7 +24704,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -26017,7 +26017,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -26679,7 +26679,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27240,7 +27240,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -27995,7 +27995,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -29962,7 +29962,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -31948,7 +31948,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -32580,7 +32580,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>

</xml_diff>